<commit_message>
removing "$" from csv
</commit_message>
<xml_diff>
--- a/source/pages/tables/GAMS engine pricing.xlsx
+++ b/source/pages/tables/GAMS engine pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VO-documentation\source\pages\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E658F97A-DE82-4DDB-993B-022F7D3BFB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F431B6F5-664C-4664-878C-729DE65524B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,16 +62,13 @@
     <t>z1d.3xlarge (92 GB RAM, 11.7 CPU) CPLEX $1.12 / h $14.00 / h $15.12 / h</t>
   </si>
   <si>
-    <t>Hourly rate</t>
+    <t>$/hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,7 +548,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -909,7 +906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -949,15 +948,15 @@
         <v>12.37</v>
       </c>
       <c r="C2">
-        <f>ROUNDUP($I2*C$6/10,0)*10</f>
+        <f t="shared" ref="C2:E4" si="0">ROUNDUP($I2*C$6/10,0)*10</f>
         <v>500</v>
       </c>
       <c r="D2">
-        <f>ROUNDUP($I2*D$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>1240</v>
       </c>
       <c r="E2">
-        <f>ROUNDUP($I2*E$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>6190</v>
       </c>
       <c r="F2" t="str">
@@ -980,19 +979,19 @@
         <v>12.739999999999998</v>
       </c>
       <c r="C3">
-        <f>ROUNDUP($I3*C$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>510</v>
       </c>
       <c r="D3">
-        <f>ROUNDUP($I3*D$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>1280</v>
       </c>
       <c r="E3">
-        <f>ROUNDUP($I3*E$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>6370</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F4" si="0">LEFT(L3,FIND(")",L3))</f>
+        <f t="shared" ref="F3:F4" si="1">LEFT(L3,FIND(")",L3))</f>
         <v>z1d.2xlarge (62 GB RAM, 7.7 CPU)</v>
       </c>
       <c r="I3">
@@ -1012,19 +1011,19 @@
         <v>13.109999999999998</v>
       </c>
       <c r="C4">
-        <f>ROUNDUP($I4*C$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>530</v>
       </c>
       <c r="D4">
-        <f>ROUNDUP($I4*D$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>1320</v>
       </c>
       <c r="E4">
-        <f>ROUNDUP($I4*E$6/10,0)*10</f>
+        <f t="shared" si="0"/>
         <v>6560</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>z1d.3xlarge (92 GB RAM, 11.7 CPU)</v>
       </c>
       <c r="I4">

</xml_diff>

<commit_message>
hourly rate - finally
</commit_message>
<xml_diff>
--- a/source/pages/tables/GAMS engine pricing.xlsx
+++ b/source/pages/tables/GAMS engine pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VO-documentation\source\pages\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F431B6F5-664C-4664-878C-729DE65524B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684868AE-1C3E-417E-A826-AE19B60CBB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
     <t>z1d.3xlarge (92 GB RAM, 11.7 CPU) CPLEX $1.12 / h $14.00 / h $15.12 / h</t>
   </si>
   <si>
-    <t>$/hour</t>
+    <t>Hourly rate</t>
   </si>
 </sst>
 </file>
@@ -907,7 +907,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,9 +943,9 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <f>I2</f>
-        <v>12.37</v>
+      <c r="B2" s="1" t="str">
+        <f>TEXT(I2,"$00.00")</f>
+        <v>$12.37</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:E4" si="0">ROUNDUP($I2*C$6/10,0)*10</f>
@@ -974,9 +974,9 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <f>I3</f>
-        <v>12.739999999999998</v>
+      <c r="B3" s="1" t="str">
+        <f t="shared" ref="B3:B4" si="1">TEXT(I3,"$00.00")</f>
+        <v>$12.74</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
@@ -991,7 +991,7 @@
         <v>6370</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F4" si="1">LEFT(L3,FIND(")",L3))</f>
+        <f t="shared" ref="F3:F4" si="2">LEFT(L3,FIND(")",L3))</f>
         <v>z1d.2xlarge (62 GB RAM, 7.7 CPU)</v>
       </c>
       <c r="I3">
@@ -1006,9 +1006,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <f>I4</f>
-        <v>13.109999999999998</v>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>$13.11</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -1023,7 +1023,7 @@
         <v>6560</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>z1d.3xlarge (92 GB RAM, 11.7 CPU)</v>
       </c>
       <c r="I4">

</xml_diff>